<commit_message>
EEst só com onda quadrada compila
</commit_message>
<xml_diff>
--- a/Arduino/teste_DAC/resultado.xlsx
+++ b/Arduino/teste_DAC/resultado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe Augusto\Google Drive\UFU\BioLab\TCC\Software\Arduino\teste_DAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B47AEF6-080C-44C5-A4B4-688E77FB05D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A183053-D225-4898-A026-34C2FD2726A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B4E05B28-0F53-4AD2-A6D3-335FCB8C68A4}"/>
   </bookViews>
@@ -25882,7 +25882,7 @@
   <dimension ref="A1:E4097"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25905,6 +25905,9 @@
       <c r="B2">
         <v>666</v>
       </c>
+      <c r="C2">
+        <v>0.54</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
@@ -25927,6 +25930,9 @@
       </c>
       <c r="B4">
         <v>668</v>
+      </c>
+      <c r="C4">
+        <v>2.74</v>
       </c>
       <c r="D4">
         <v>3</v>

</xml_diff>